<commit_message>
Minor adjustments in mapping xlsx Concern and Contact
</commit_message>
<xml_diff>
--- a/Mappings/Concern - STU3.xlsx
+++ b/Mappings/Concern - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="26835" windowHeight="11325"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="26835" windowHeight="11325" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OverdrachtConcern" sheetId="1" r:id="rId1"/>
@@ -1002,7 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Adjusted mapping of ConcernLabel based on issue MSFOC-2
</commit_message>
<xml_diff>
--- a/Mappings/Concern - STU3.xlsx
+++ b/Mappings/Concern - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="26835" windowHeight="11325" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="26835" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="OverdrachtConcern" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="ProbleemStatusCodelijst" sheetId="3" r:id="rId3"/>
     <sheet name="ProbleemNaamCodelijst" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="89">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -64,9 +64,6 @@
     <t>Toelichting</t>
   </si>
   <si>
-    <t>Condition (problem)</t>
-  </si>
-  <si>
     <t>Condition.category</t>
   </si>
   <si>
@@ -238,16 +235,10 @@
     <t>FHIR</t>
   </si>
   <si>
-    <t>Condition.code.text</t>
-  </si>
-  <si>
     <t>Condition.clinicalStatus.extension</t>
   </si>
   <si>
     <t>Condition.note</t>
-  </si>
-  <si>
-    <t>Will be removed from the ZIB</t>
   </si>
   <si>
     <r>
@@ -311,6 +302,12 @@
   </si>
   <si>
     <t>FHIR valueset binding Required. ZIB maps to FHIR ValueSet FHIR is more detailed.</t>
+  </si>
+  <si>
+    <t>EpisodeOfCare.type.text</t>
+  </si>
+  <si>
+    <t>Condition (problem) + EpisodeOfCare</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1050,7 +1047,7 @@
       <c r="H2" s="42"/>
       <c r="I2" s="43"/>
       <c r="J2" s="23" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="K2" s="23"/>
     </row>
@@ -1071,11 +1068,9 @@
       <c r="H3" s="16"/>
       <c r="I3" s="3"/>
       <c r="J3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K3" s="35" t="s">
-        <v>76</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="4">
@@ -1106,15 +1101,15 @@
       <c r="E5" s="9"/>
       <c r="F5" s="14"/>
       <c r="G5" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="4"/>
       <c r="J5" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="25.5">
@@ -1128,15 +1123,15 @@
       </c>
       <c r="E6" s="14"/>
       <c r="G6" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="19"/>
       <c r="J6" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1151,12 +1146,12 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="19"/>
       <c r="J7" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" s="30"/>
     </row>
@@ -1172,14 +1167,14 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="17"/>
       <c r="J8" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1194,12 +1189,12 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="21"/>
       <c r="J9" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K9" s="30"/>
     </row>
@@ -1215,12 +1210,12 @@
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="6"/>
       <c r="J10" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K10" s="27"/>
     </row>
@@ -1264,16 +1259,16 @@
   <sheetData>
     <row r="2" spans="1:5">
       <c r="A2" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="C2" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="D2" s="32" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>23</v>
       </c>
       <c r="E2" s="32"/>
     </row>
@@ -1285,108 +1280,108 @@
         <v>55607006</v>
       </c>
       <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
         <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>64572001</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>282291009</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>418799008</v>
       </c>
       <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>404684003</v>
       </c>
       <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>409586006</v>
       </c>
       <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
         <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>248536006</v>
       </c>
       <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>116223007</v>
       </c>
       <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
         <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="24" spans="5:9">
@@ -1406,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1421,74 +1416,74 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="44"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>38</v>
-      </c>
       <c r="E3" s="33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="33" t="s">
+      <c r="D5" s="33" t="s">
         <v>46</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>47</v>
       </c>
       <c r="E5" s="33"/>
     </row>
@@ -1498,136 +1493,136 @@
     </row>
     <row r="15" spans="1:9" s="32" customFormat="1">
       <c r="A15" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="32" customFormat="1">
       <c r="A16" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="C16" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="D16" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="32" t="s">
-        <v>23</v>
-      </c>
       <c r="G16" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="I16" s="32" t="s">
         <v>35</v>
-      </c>
-      <c r="I16" s="32" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>55561003</v>
       </c>
       <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" t="s">
         <v>37</v>
       </c>
-      <c r="H17" t="s">
-        <v>38</v>
-      </c>
       <c r="I17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>73425007</v>
       </c>
       <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>413322009</v>
       </c>
       <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
         <v>25</v>
       </c>
-      <c r="D19" t="s">
-        <v>26</v>
-      </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="E20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" t="s">
         <v>40</v>
-      </c>
-      <c r="I20" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="G21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1656,100 +1651,100 @@
   <sheetData>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
         <v>57</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>58</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
         <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
         <v>63</v>
-      </c>
-      <c r="C11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
         <v>65</v>
-      </c>
-      <c r="C12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
         <v>67</v>
-      </c>
-      <c r="C13" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
         <v>69</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>